<commit_message>
sua dong ho dem nguoc, sua tim kiem thong tin de thi
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/abc.xlsx
+++ b/src/main/resources/static/excel/abc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t>GiaiThich</t>
   </si>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,9 +530,201 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 F2:F4 H2:H4 J2:J4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10 F2:F10 H2:H10 J2:J10">
       <formula1>"0,1"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">

</xml_diff>

<commit_message>
Revert "sua dong ho dem nguoc, sua tim kiem thong tin de thi"
This reverts commit 225e229892c60b19e56a037608020a2a17b980c5.
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/abc.xlsx
+++ b/src/main/resources/static/excel/abc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>GiaiThich</t>
   </si>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,201 +530,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10 F2:F10 H2:H10 J2:J10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 F2:F4 H2:H4 J2:J4">
       <formula1>"0,1"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">

</xml_diff>

<commit_message>
sua giao dien de thi, them excel
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/abc.xlsx
+++ b/src/main/resources/static/excel/abc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t>GiaiThich</t>
   </si>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,9 +530,201 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 F2:F4 H2:H4 J2:J4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10 F2:F10 H2:H10 J2:J10">
       <formula1>"0,1"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">

</xml_diff>

<commit_message>
Hoàn thành bài làm, chỉnh sửa ảnh đề thi, ảnh đại diện
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/abc.xlsx
+++ b/src/main/resources/static/excel/abc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF6E88E-C644-4EB4-B693-3B594E2858C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="4584"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>GiaiThich</t>
   </si>
@@ -43,43 +43,43 @@
     <t>noidung_phuong_an2</t>
   </si>
   <si>
-    <t>A, Con mèo có trước hay con chó có trước</t>
-  </si>
-  <si>
-    <t>B, Con mèo có trước hay con chó có trước</t>
-  </si>
-  <si>
-    <t>C, Con mèo có trước hay con chó có trước</t>
-  </si>
-  <si>
-    <t>D, Con mèo có trước hay con chó có trước</t>
-  </si>
-  <si>
-    <t>hai</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>bon</t>
-  </si>
-  <si>
-    <t>asdf2222</t>
-  </si>
-  <si>
-    <t>asdf333</t>
-  </si>
-  <si>
-    <t>asdf444</t>
-  </si>
-  <si>
-    <t>asdf</t>
+    <t>Có công mài sắt có ngày nên …..</t>
+  </si>
+  <si>
+    <t>kim</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Người</t>
+  </si>
+  <si>
+    <t>Dao</t>
+  </si>
+  <si>
+    <t>Kéo</t>
+  </si>
+  <si>
+    <t>Uống nước nhớ ….</t>
+  </si>
+  <si>
+    <t>Nguồn</t>
+  </si>
+  <si>
+    <t>Nhà sản xuất</t>
+  </si>
+  <si>
+    <t>Quả</t>
+  </si>
+  <si>
+    <t>Cây</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,11 +394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,31 +446,31 @@
     </row>
     <row r="2" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -478,74 +478,48 @@
     </row>
     <row r="3" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
+    <row r="4" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 F2:F4 H2:H4 J2:J4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 F2:F4 H2:H4 J2:J4">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>